<commit_message>
updated with multiple dynamic input
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,14 +501,74 @@
           <t>Prakash</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="B5" t="n">
+        <v>101</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>17:50:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Prakash</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>101</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>18:01:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Prakash</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>101</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18:14:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Prakash</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>101</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>18:18:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kolass</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>18:18:46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
4th step updated working fine
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,114 +461,69 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17:48:29</t>
+          <t>21:40:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kolass</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>17:49:08</t>
+          <t>21:41:06</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Prakash</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>17:49:28</t>
+          <t>21:42:52</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Prakash</t>
+          <t>Kolass</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>17:50:30</t>
+          <t>21:43:04</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Prakash</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>101</v>
+          <t>Mary</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>18:01:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Prakash</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>101</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>18:14:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Prakash</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>101</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>18:18:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Kolass</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>18:18:46</t>
+          <t>21:43:04</t>
         </is>
       </c>
     </row>

</xml_diff>